<commit_message>
created maven project for selenium
</commit_message>
<xml_diff>
--- a/shopizer_Signin_Page_Isha_Agrawal.xlsx
+++ b/shopizer_Signin_Page_Isha_Agrawal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Mini project\git track\Shopizer\Shopizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C170684A-FC89-4C5A-A6E5-338B3125FBD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB94DC-F12F-46C8-8AB9-6F0C355899F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="253" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,12 +172,6 @@
     <t>Enter the password in the password field</t>
   </si>
   <si>
-    <t>SC_01_TC_14</t>
-  </si>
-  <si>
-    <t>SC_01_TC_15</t>
-  </si>
-  <si>
     <t>Check the Sign in functionality</t>
   </si>
   <si>
@@ -311,6 +305,12 @@
   </si>
   <si>
     <t>User must be Signed in and navigated to the account's Dashboard</t>
+  </si>
+  <si>
+    <t>SC_01_TC_11</t>
+  </si>
+  <si>
+    <t>SC_01_TC_12</t>
   </si>
 </sst>
 </file>
@@ -885,10 +885,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>14</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>24</v>
@@ -921,10 +921,10 @@
       <c r="B5" s="6"/>
       <c r="C5" s="14"/>
       <c r="D5" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -942,7 +942,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="8"/>
       <c r="E7" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -950,7 +950,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="15"/>
       <c r="E8" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -977,7 +977,7 @@
       <c r="C11" s="26"/>
       <c r="D11" s="8"/>
       <c r="E11" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -986,7 +986,7 @@
       <c r="C12" s="16"/>
       <c r="D12" s="8"/>
       <c r="E12" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -995,7 +995,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1004,7 +1004,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1013,7 +1013,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="8"/>
       <c r="E15" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1022,7 +1022,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="8"/>
       <c r="E16" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,7 +1204,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>19</v>
@@ -1232,7 +1232,7 @@
       <c r="A4" s="21"/>
       <c r="B4" s="14"/>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1246,7 +1246,7 @@
       <c r="A5" s="22"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -1276,7 +1276,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>21</v>
@@ -1306,7 +1306,7 @@
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1321,7 +1321,7 @@
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1352,7 +1352,7 @@
         <v>18</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>21</v>
@@ -1382,7 +1382,7 @@
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1397,7 +1397,7 @@
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1413,7 +1413,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>14</v>
@@ -1422,13 +1422,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>21</v>
@@ -1461,7 +1461,7 @@
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -1479,7 +1479,7 @@
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -1507,16 +1507,16 @@
         <v>1</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>42</v>
@@ -1550,7 +1550,7 @@
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -1565,7 +1565,7 @@
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -1581,7 +1581,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>14</v>
@@ -1590,13 +1590,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" s="14" t="s">
         <v>21</v>
@@ -1617,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1630,7 +1630,7 @@
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -1645,7 +1645,7 @@
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -1661,7 +1661,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>14</v>
@@ -1670,13 +1670,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H26" s="14" t="s">
         <v>21</v>
@@ -1700,7 +1700,7 @@
         <v>38</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -1712,13 +1712,13 @@
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28" s="14">
         <v>3</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1731,7 +1731,7 @@
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -1821,13 +1821,13 @@
         <v>1</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>21</v>
@@ -1851,7 +1851,7 @@
         <v>38</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -1863,13 +1863,13 @@
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D37" s="14">
         <v>3</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -1882,7 +1882,7 @@
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -1972,14 +1972,14 @@
         <v>1</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F44" s="14" t="str">
         <f>$F$35</f>
         <v>Email ID: ishaagraawal2000@gmail.com</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H44" s="14" t="s">
         <v>21</v>
@@ -2000,7 +2000,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
@@ -2013,7 +2013,7 @@
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -2028,7 +2028,7 @@
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
@@ -2044,7 +2044,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>14</v>
@@ -2053,13 +2053,13 @@
         <v>1</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>19</v>
@@ -2080,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
@@ -2093,7 +2093,7 @@
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
@@ -2108,7 +2108,7 @@
       <c r="A51" s="14"/>
       <c r="B51" s="6"/>
       <c r="C51" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -2119,270 +2119,189 @@
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
     </row>
-    <row r="52" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
+      <c r="C54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A56" s="14"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
+      <c r="C56" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C58"/>
-    </row>
-    <row r="60" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+      <c r="C58" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="29" t="s">
+      <c r="B61" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="14">
+        <v>1</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C62" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="14">
+        <v>2</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C63" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J60" s="14"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C61" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="1">
-        <v>2</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C62" t="s">
+      <c r="D63" s="14">
+        <v>3</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F63" s="14"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C64" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C63" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="1">
-        <v>1</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C65" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="1">
-        <v>2</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C66" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C67" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C69" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="14">
-        <v>2</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C70" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="14">
-        <v>3</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F70" s="14"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C71" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="30"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="30"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="30"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="30"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="30"/>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="30"/>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="30"/>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>